<commit_message>
Updates to Form Values
</commit_message>
<xml_diff>
--- a/batch_update_documentation/Rationalising_Item_Form_values.xlsx
+++ b/batch_update_documentation/Rationalising_Item_Form_values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\British Library\bl github group\bl_github_clones\idp-data-issues\batch_update_documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD591C85-9080-463B-BB0E-103FFF3F3C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D635E0-62DE-4CAD-B902-7905568FF035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14604" yWindow="6204" windowWidth="25032" windowHeight="18600" xr2:uid="{C1BD5365-450B-4DF4-BFDD-736E06AB95DB}"/>
+    <workbookView xWindow="17832" yWindow="6960" windowWidth="25032" windowHeight="18600" xr2:uid="{C1BD5365-450B-4DF4-BFDD-736E06AB95DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Ths Excel sheet will be used to define a TSV for batch update of Form values</t>
   </si>
@@ -45,13 +45,61 @@
   </si>
   <si>
     <t>Rationalising_Item_Form_values.xlsx</t>
+  </si>
+  <si>
+    <t>digital photograph</t>
+  </si>
+  <si>
+    <t>FORM001250</t>
+  </si>
+  <si>
+    <t>BL</t>
+  </si>
+  <si>
+    <t>BLS</t>
+  </si>
+  <si>
+    <t>BNF</t>
+  </si>
+  <si>
+    <t>-Fotografi-</t>
+  </si>
+  <si>
+    <t>FORM002100</t>
+  </si>
+  <si>
+    <t>SMVK-EM</t>
+  </si>
+  <si>
+    <t>fotografi</t>
+  </si>
+  <si>
+    <t>FORM002793</t>
+  </si>
+  <si>
+    <t>photography</t>
+  </si>
+  <si>
+    <t>FORM002795</t>
+  </si>
+  <si>
+    <t>Photogravure</t>
+  </si>
+  <si>
+    <t>FORM002020</t>
+  </si>
+  <si>
+    <t>MAP ALL OF THE FOLLOWING TO FORM001250</t>
+  </si>
+  <si>
+    <t>WHAT TO DO FOR PARTNER SITES? No good modifyinh if Sync will overwrite</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +115,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -76,9 +130,33 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -88,9 +166,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,26 +489,135 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC8EA5C5-E56F-4438-98D0-7ECA2217BD33}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="31.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2676</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>